<commit_message>
completed debugging of data.py
</commit_message>
<xml_diff>
--- a/given_excel.xlsx
+++ b/given_excel.xlsx
@@ -529,6 +529,44 @@
           <t>https://www.zillow.com/homedetails/6-Standish-Cir-Andover-MA-01810/56034004_zpid/</t>
         </is>
       </c>
+      <c r="K2" t="n">
+        <v>917100</v>
+      </c>
+      <c r="L2" t="n">
+        <v>752900</v>
+      </c>
+      <c r="M2" t="n">
+        <v>2024</v>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O2" t="n">
+        <v>2148</v>
+      </c>
+      <c r="P2" t="n">
+        <v>1964</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>0.4699954086317722</v>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>Forced air,Gas</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -575,6 +613,44 @@
           <t>https://www.zillow.com/homedetails/150-Traincroft-NW-Medford-MA-02155/56277119_zpid/</t>
         </is>
       </c>
+      <c r="K3" t="n">
+        <v>1216400</v>
+      </c>
+      <c r="L3" t="n">
+        <v>931700</v>
+      </c>
+      <c r="M3" t="n">
+        <v>2024</v>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>2012-07-24</t>
+        </is>
+      </c>
+      <c r="O3" t="n">
+        <v>2258</v>
+      </c>
+      <c r="P3" t="n">
+        <v>1929</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>7590</v>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>Square Feet</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>Electric Baseboard,Steam,Natural Gas</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -621,6 +697,44 @@
           <t>https://www.zillow.com/homedetails/24-Dean-Rd-Wayland-MA-01778/57127108_zpid/</t>
         </is>
       </c>
+      <c r="K4" t="n">
+        <v>1035600</v>
+      </c>
+      <c r="L4" t="n">
+        <v>831600</v>
+      </c>
+      <c r="M4" t="n">
+        <v>2024</v>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>2008-06-27</t>
+        </is>
+      </c>
+      <c r="O4" t="n">
+        <v>1668</v>
+      </c>
+      <c r="P4" t="n">
+        <v>1952</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>0.5799816345270891</v>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>Forced air,Gas</t>
+        </is>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -667,6 +781,50 @@
           <t>https://www.zillow.com/homedetails/173-Bay-Rd-Harwich-MA-02645/186993999_zpid/</t>
         </is>
       </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="L5" t="n">
+        <v>995700</v>
+      </c>
+      <c r="M5" t="n">
+        <v>2024</v>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>1999-04-09</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="Q5" t="n">
+        <v>0.9199954086317723</v>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -713,6 +871,44 @@
           <t>https://www.zillow.com/homedetails/1-Ladyslipper-Ln-Hadley-MA-01035/57015531_zpid/</t>
         </is>
       </c>
+      <c r="K6" t="n">
+        <v>652800</v>
+      </c>
+      <c r="L6" t="n">
+        <v>505800</v>
+      </c>
+      <c r="M6" t="n">
+        <v>2024</v>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>1987-09-01</t>
+        </is>
+      </c>
+      <c r="O6" t="n">
+        <v>2366</v>
+      </c>
+      <c r="P6" t="n">
+        <v>1987</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>Other,Oil</t>
+        </is>
+      </c>
+      <c r="T6" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -759,6 +955,44 @@
           <t>https://www.zillow.com/homedetails/170-Kilkore-Dr-Hyannis-MA-02601/55846500_zpid/</t>
         </is>
       </c>
+      <c r="K7" t="n">
+        <v>761800</v>
+      </c>
+      <c r="L7" t="n">
+        <v>622300</v>
+      </c>
+      <c r="M7" t="n">
+        <v>2024</v>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>2008-10-16</t>
+        </is>
+      </c>
+      <c r="O7" t="n">
+        <v>1612</v>
+      </c>
+      <c r="P7" t="n">
+        <v>2000</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>9583</v>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>Square Feet</t>
+        </is>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>Forced air,Gas</t>
+        </is>
+      </c>
+      <c r="T7" t="inlineStr">
+        <is>
+          <t>Central</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -805,6 +1039,44 @@
           <t>https://www.zillow.com/homedetails/39-Stevens-St-Stoneham-MA-02180/56336960_zpid/</t>
         </is>
       </c>
+      <c r="K8" t="n">
+        <v>805200</v>
+      </c>
+      <c r="L8" t="n">
+        <v>655300</v>
+      </c>
+      <c r="M8" t="n">
+        <v>2024</v>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>1996-05-24</t>
+        </is>
+      </c>
+      <c r="O8" t="n">
+        <v>1333</v>
+      </c>
+      <c r="P8" t="n">
+        <v>1930</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>0.3994490358126722</v>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="S8" t="inlineStr">
+        <is>
+          <t>Heat pump,Electric,Solar</t>
+        </is>
+      </c>
+      <c r="T8" t="inlineStr">
+        <is>
+          <t>Central,Solar</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -851,6 +1123,44 @@
           <t>https://www.zillow.com/homedetails/17-Milbery-Ln-Pembroke-MA-02359/57536844_zpid/</t>
         </is>
       </c>
+      <c r="K9" t="n">
+        <v>907000</v>
+      </c>
+      <c r="L9" t="n">
+        <v>736800</v>
+      </c>
+      <c r="M9" t="n">
+        <v>2024</v>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O9" t="n">
+        <v>2520</v>
+      </c>
+      <c r="P9" t="n">
+        <v>1989</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>1.069995408631772</v>
+      </c>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="S9" t="inlineStr">
+        <is>
+          <t>Other,Oil</t>
+        </is>
+      </c>
+      <c r="T9" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -897,6 +1207,44 @@
           <t>https://www.zillow.com/homedetails/16-Harris-Ln-Harvard-MA-01451/173940899_zpid/</t>
         </is>
       </c>
+      <c r="K10" t="n">
+        <v>1219200</v>
+      </c>
+      <c r="L10" t="n">
+        <v>985500</v>
+      </c>
+      <c r="M10" t="n">
+        <v>2024</v>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>2015-08-14</t>
+        </is>
+      </c>
+      <c r="O10" t="n">
+        <v>3564</v>
+      </c>
+      <c r="P10" t="n">
+        <v>2000</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>4.479981634527089</v>
+      </c>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="S10" t="inlineStr">
+        <is>
+          <t>Forced air,Heat pump,Stove,Oil,Solar,Wood / Pellet</t>
+        </is>
+      </c>
+      <c r="T10" t="inlineStr">
+        <is>
+          <t>Central,Solar</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -943,6 +1291,44 @@
           <t>https://www.zillow.com/homedetails/21-White-Oaks-Rd-Williamstown-MA-01267/56819688_zpid/</t>
         </is>
       </c>
+      <c r="K11" t="n">
+        <v>409300</v>
+      </c>
+      <c r="L11" t="n">
+        <v>332300</v>
+      </c>
+      <c r="M11" t="n">
+        <v>2024</v>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O11" t="n">
+        <v>1958</v>
+      </c>
+      <c r="P11" t="n">
+        <v>1950</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>0.2899908172635445</v>
+      </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="S11" t="inlineStr">
+        <is>
+          <t>Forced air,Oil</t>
+        </is>
+      </c>
+      <c r="T11" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
@@ -989,6 +1375,44 @@
           <t>https://www.zillow.com/homedetails/20-Overlook-Dr-East-Longmeadow-MA-01028/56171418_zpid/</t>
         </is>
       </c>
+      <c r="K12" t="n">
+        <v>486900</v>
+      </c>
+      <c r="L12" t="n">
+        <v>422700</v>
+      </c>
+      <c r="M12" t="n">
+        <v>2024</v>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>2017-08-21</t>
+        </is>
+      </c>
+      <c r="O12" t="n">
+        <v>1656</v>
+      </c>
+      <c r="P12" t="n">
+        <v>1994</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>0.6699954086317723</v>
+      </c>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="S12" t="inlineStr">
+        <is>
+          <t>Forced air,Oil</t>
+        </is>
+      </c>
+      <c r="T12" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
@@ -1035,6 +1459,44 @@
           <t>https://www.zillow.com/homedetails/58-Linda-Ave-Framingham-MA-01701/165985595_zpid/</t>
         </is>
       </c>
+      <c r="K13" t="n">
+        <v>698200</v>
+      </c>
+      <c r="L13" t="n">
+        <v>557400</v>
+      </c>
+      <c r="M13" t="n">
+        <v>2024</v>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>2013-09-16</t>
+        </is>
+      </c>
+      <c r="O13" t="n">
+        <v>1356</v>
+      </c>
+      <c r="P13" t="n">
+        <v>1954</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>10018</v>
+      </c>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>Square Feet</t>
+        </is>
+      </c>
+      <c r="S13" t="inlineStr">
+        <is>
+          <t>Gas</t>
+        </is>
+      </c>
+      <c r="T13" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
@@ -1081,6 +1543,44 @@
           <t>https://www.zillow.com/homedetails/19-Holly-Cir-Easthampton-MA-01027/57009823_zpid/</t>
         </is>
       </c>
+      <c r="K14" t="n">
+        <v>792800</v>
+      </c>
+      <c r="L14" t="n">
+        <v>680500</v>
+      </c>
+      <c r="M14" t="n">
+        <v>2024</v>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>2017-03-10</t>
+        </is>
+      </c>
+      <c r="O14" t="n">
+        <v>3265</v>
+      </c>
+      <c r="P14" t="n">
+        <v>1999</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>1.089990817263545</v>
+      </c>
+      <c r="R14" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="S14" t="inlineStr">
+        <is>
+          <t>Forced air,Stove,Gas</t>
+        </is>
+      </c>
+      <c r="T14" t="inlineStr">
+        <is>
+          <t>Central</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
@@ -1127,6 +1627,44 @@
           <t>https://www.zillow.com/homedetails/31-E-Sound-Ln-Tisbury-MA-02568/56900325_zpid/</t>
         </is>
       </c>
+      <c r="K15" t="n">
+        <v>4478700</v>
+      </c>
+      <c r="L15" t="n">
+        <v>3764200</v>
+      </c>
+      <c r="M15" t="n">
+        <v>2024</v>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>2016-10-28</t>
+        </is>
+      </c>
+      <c r="O15" t="n">
+        <v>2672</v>
+      </c>
+      <c r="P15" t="n">
+        <v>1996</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>3.569995408631772</v>
+      </c>
+      <c r="R15" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="S15" t="inlineStr">
+        <is>
+          <t>Forced air,Gas</t>
+        </is>
+      </c>
+      <c r="T15" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
@@ -1173,6 +1711,44 @@
           <t>https://www.zillow.com/homedetails/156-Standish-Rd-Needham-MA-02492/57478769_zpid/</t>
         </is>
       </c>
+      <c r="K16" t="n">
+        <v>1559500</v>
+      </c>
+      <c r="L16" t="n">
+        <v>1099000</v>
+      </c>
+      <c r="M16" t="n">
+        <v>2024</v>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>2001-08-06</t>
+        </is>
+      </c>
+      <c r="O16" t="n">
+        <v>2612</v>
+      </c>
+      <c r="P16" t="n">
+        <v>1974</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>0.2599862258953168</v>
+      </c>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="S16" t="inlineStr">
+        <is>
+          <t>Forced air,Gas</t>
+        </is>
+      </c>
+      <c r="T16" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
@@ -1219,6 +1795,44 @@
           <t>https://www.zillow.com/homedetails/18-Bartkus-Farm-Concord-MA-01742/166021417_zpid/</t>
         </is>
       </c>
+      <c r="K17" t="n">
+        <v>1916600</v>
+      </c>
+      <c r="L17" t="n">
+        <v>1622300</v>
+      </c>
+      <c r="M17" t="n">
+        <v>2024</v>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>2006-07-14</t>
+        </is>
+      </c>
+      <c r="O17" t="n">
+        <v>4964</v>
+      </c>
+      <c r="P17" t="n">
+        <v>1991</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="S17" t="inlineStr">
+        <is>
+          <t>Electric</t>
+        </is>
+      </c>
+      <c r="T17" t="inlineStr">
+        <is>
+          <t>Central</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
@@ -1265,6 +1879,44 @@
           <t>https://www.zillow.com/homedetails/17-Mello-St-East-Falmouth-MA-02536/55885097_zpid/</t>
         </is>
       </c>
+      <c r="K18" t="n">
+        <v>544200</v>
+      </c>
+      <c r="L18" t="n">
+        <v>396100</v>
+      </c>
+      <c r="M18" t="n">
+        <v>2024</v>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>2008-03-19</t>
+        </is>
+      </c>
+      <c r="O18" t="n">
+        <v>1040</v>
+      </c>
+      <c r="P18" t="n">
+        <v>1958</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>10018</v>
+      </c>
+      <c r="R18" t="inlineStr">
+        <is>
+          <t>Square Feet</t>
+        </is>
+      </c>
+      <c r="S18" t="inlineStr">
+        <is>
+          <t>Other,Oil</t>
+        </is>
+      </c>
+      <c r="T18" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
@@ -1311,6 +1963,44 @@
           <t>https://www.zillow.com/homedetails/198-W-River-St-Upton-MA-01568/173952657_zpid/</t>
         </is>
       </c>
+      <c r="K19" t="n">
+        <v>782600</v>
+      </c>
+      <c r="L19" t="n">
+        <v>645600</v>
+      </c>
+      <c r="M19" t="n">
+        <v>2024</v>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O19" t="n">
+        <v>2936</v>
+      </c>
+      <c r="P19" t="n">
+        <v>1992</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>1.839990817263545</v>
+      </c>
+      <c r="R19" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="S19" t="inlineStr">
+        <is>
+          <t>Oil</t>
+        </is>
+      </c>
+      <c r="T19" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
@@ -1357,6 +2047,44 @@
           <t>https://www.zillow.com/homedetails/298-Heaths-Bridge-Rd-Concord-MA-01742/166021031_zpid/</t>
         </is>
       </c>
+      <c r="K20" t="n">
+        <v>1358300</v>
+      </c>
+      <c r="L20" t="n">
+        <v>1153100</v>
+      </c>
+      <c r="M20" t="n">
+        <v>2024</v>
+      </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O20" t="n">
+        <v>2020</v>
+      </c>
+      <c r="P20" t="n">
+        <v>1953</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>1.109986225895317</v>
+      </c>
+      <c r="R20" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="S20" t="inlineStr">
+        <is>
+          <t>Oil</t>
+        </is>
+      </c>
+      <c r="T20" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
@@ -1403,6 +2131,44 @@
           <t>https://www.zillow.com/homedetails/66-Milk-St-Nantucket-MA-02554/56544257_zpid/</t>
         </is>
       </c>
+      <c r="K21" t="n">
+        <v>3081500</v>
+      </c>
+      <c r="L21" t="n">
+        <v>1727200</v>
+      </c>
+      <c r="M21" t="n">
+        <v>2024</v>
+      </c>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>2018-09-20</t>
+        </is>
+      </c>
+      <c r="O21" t="n">
+        <v>2844</v>
+      </c>
+      <c r="P21" t="n">
+        <v>2000</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>0.463682277318641</v>
+      </c>
+      <c r="R21" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="S21" t="inlineStr">
+        <is>
+          <t>Solar</t>
+        </is>
+      </c>
+      <c r="T21" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
@@ -1449,6 +2215,44 @@
           <t>https://www.zillow.com/homedetails/116-Charlton-St-Oxford-MA-01540/60027614_zpid/</t>
         </is>
       </c>
+      <c r="K22" t="n">
+        <v>497900</v>
+      </c>
+      <c r="L22" t="n">
+        <v>429200</v>
+      </c>
+      <c r="M22" t="n">
+        <v>2024</v>
+      </c>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O22" t="n">
+        <v>1714</v>
+      </c>
+      <c r="P22" t="n">
+        <v>1961</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="R22" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="S22" t="inlineStr">
+        <is>
+          <t>Other,Electric</t>
+        </is>
+      </c>
+      <c r="T22" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
@@ -1495,6 +2299,44 @@
           <t>https://www.zillow.com/homedetails/262-Sheep-Pond-Dr-Brewster-MA-02631/56767509_zpid/</t>
         </is>
       </c>
+      <c r="K23" t="n">
+        <v>1900300</v>
+      </c>
+      <c r="L23" t="n">
+        <v>1426800</v>
+      </c>
+      <c r="M23" t="n">
+        <v>2024</v>
+      </c>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>2006-09-20</t>
+        </is>
+      </c>
+      <c r="O23" t="n">
+        <v>2849</v>
+      </c>
+      <c r="P23" t="n">
+        <v>2007</v>
+      </c>
+      <c r="Q23" t="n">
+        <v>0.4683195592286502</v>
+      </c>
+      <c r="R23" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="S23" t="inlineStr">
+        <is>
+          <t>Baseboard,Gas</t>
+        </is>
+      </c>
+      <c r="T23" t="inlineStr">
+        <is>
+          <t>Central</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
@@ -1541,6 +2383,44 @@
           <t>https://www.zillow.com/homedetails/67-Gorwin-Dr-Hanson-MA-02341/184281722_zpid/</t>
         </is>
       </c>
+      <c r="K24" t="n">
+        <v>670200</v>
+      </c>
+      <c r="L24" t="n">
+        <v>534500</v>
+      </c>
+      <c r="M24" t="n">
+        <v>2024</v>
+      </c>
+      <c r="N24" t="inlineStr">
+        <is>
+          <t>2016-03-29</t>
+        </is>
+      </c>
+      <c r="O24" t="n">
+        <v>1858</v>
+      </c>
+      <c r="P24" t="n">
+        <v>1968</v>
+      </c>
+      <c r="Q24" t="n">
+        <v>0.6899908172635445</v>
+      </c>
+      <c r="R24" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="S24" t="inlineStr">
+        <is>
+          <t>Gas</t>
+        </is>
+      </c>
+      <c r="T24" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
@@ -1587,6 +2467,44 @@
           <t>https://www.zillow.com/homedetails/9-Samuel-Parlin-Dr-Acton-MA-01720/57031578_zpid/</t>
         </is>
       </c>
+      <c r="K25" t="n">
+        <v>1235700</v>
+      </c>
+      <c r="L25" t="n">
+        <v>922500</v>
+      </c>
+      <c r="M25" t="n">
+        <v>2024</v>
+      </c>
+      <c r="N25" t="inlineStr">
+        <is>
+          <t>2009-08-19</t>
+        </is>
+      </c>
+      <c r="O25" t="n">
+        <v>3541</v>
+      </c>
+      <c r="P25" t="n">
+        <v>1971</v>
+      </c>
+      <c r="Q25" t="n">
+        <v>0.9366620752984389</v>
+      </c>
+      <c r="R25" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="S25" t="inlineStr">
+        <is>
+          <t>Other,Gas</t>
+        </is>
+      </c>
+      <c r="T25" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
@@ -1633,6 +2551,44 @@
           <t>https://www.zillow.com/homedetails/34-Hoover-Ave-Brockton-MA-02301/57161799_zpid/</t>
         </is>
       </c>
+      <c r="K26" t="n">
+        <v>621400</v>
+      </c>
+      <c r="L26" t="n">
+        <v>462900</v>
+      </c>
+      <c r="M26" t="n">
+        <v>2024</v>
+      </c>
+      <c r="N26" t="inlineStr">
+        <is>
+          <t>2005-06-14</t>
+        </is>
+      </c>
+      <c r="O26" t="n">
+        <v>2342</v>
+      </c>
+      <c r="P26" t="n">
+        <v>1987</v>
+      </c>
+      <c r="Q26" t="n">
+        <v>0.2514003673094582</v>
+      </c>
+      <c r="R26" t="inlineStr">
+        <is>
+          <t>Acres</t>
+        </is>
+      </c>
+      <c r="S26" t="inlineStr">
+        <is>
+          <t>Other,Gas</t>
+        </is>
+      </c>
+      <c r="T26" t="inlineStr">
+        <is>
+          <t>Central,Solar</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
@@ -10247,6 +11203,44 @@
       <c r="J210" t="inlineStr">
         <is>
           <t>https://www.zillow.com/homedetails/45-July-St-Lowell-MA-01850/56511098_zpid/</t>
+        </is>
+      </c>
+      <c r="K210" t="n">
+        <v>536900</v>
+      </c>
+      <c r="L210" t="n">
+        <v>400700</v>
+      </c>
+      <c r="M210" t="n">
+        <v>2024</v>
+      </c>
+      <c r="N210" t="inlineStr">
+        <is>
+          <t>2022-06-17</t>
+        </is>
+      </c>
+      <c r="O210" t="n">
+        <v>1716</v>
+      </c>
+      <c r="P210" t="n">
+        <v>1930</v>
+      </c>
+      <c r="Q210" t="n">
+        <v>6969.6</v>
+      </c>
+      <c r="R210" t="inlineStr">
+        <is>
+          <t>Square Feet</t>
+        </is>
+      </c>
+      <c r="S210" t="inlineStr">
+        <is>
+          <t>Electric Baseboard,Steam,Natural Gas</t>
+        </is>
+      </c>
+      <c r="T210" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>

</xml_diff>